<commit_message>
Adding RPI system test inside
</commit_message>
<xml_diff>
--- a/docs/System_Test_Report_template.xlsx
+++ b/docs/System_Test_Report_template.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27830"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83CC02D9-6D26-4B00-A73F-07BC6499151C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overall Test Report" sheetId="2" r:id="rId1"/>
     <sheet name="Test Cases &amp; Results" sheetId="1" r:id="rId2"/>
     <sheet name="Enums" sheetId="3" state="hidden" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -20,6 +21,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="58">
   <si>
     <t>Total Test Cases</t>
   </si>
@@ -83,25 +86,130 @@
     <t>Low Impact</t>
   </si>
   <si>
-    <t>Test that the water heater is activated if the water temperature is &lt; 100 Deg C</t>
-  </si>
-  <si>
-    <t>Water temperature is &lt; 100 Deg C</t>
-  </si>
-  <si>
-    <t>From the LCD main menu, select the option "Black Coffee"</t>
-  </si>
-  <si>
-    <t>-Heating element is activated when water temperature is &lt; 100 Deg C</t>
-  </si>
-  <si>
-    <t>REQ-06</t>
+    <t>REQ-</t>
+  </si>
+  <si>
+    <t>REQ-07</t>
+  </si>
+  <si>
+    <t>Test that Pi is able to scan barcodes using Camera</t>
+  </si>
+  <si>
+    <t>Barcode is placed in reasonable distance from the Pi and is surrounded by a white background in the image</t>
+  </si>
+  <si>
+    <t>Point camera towards barcode with minimal movement</t>
+  </si>
+  <si>
+    <t>Barcode informartion is printed on terminal</t>
+  </si>
+  <si>
+    <t>REQ-09</t>
+  </si>
+  <si>
+    <t>Test that LCD displays running total</t>
+  </si>
+  <si>
+    <t>Item/Items are scanned</t>
+  </si>
+  <si>
+    <t>Scan an item using PiCam</t>
+  </si>
+  <si>
+    <t>Total price is displayed on LCD</t>
+  </si>
+  <si>
+    <t>REQ-10</t>
+  </si>
+  <si>
+    <t>Test that pressing '#' will exit the scanning process</t>
+  </si>
+  <si>
+    <t>nil</t>
+  </si>
+  <si>
+    <t>Code is executing scanning portion</t>
+  </si>
+  <si>
+    <t>Press '#' on LCD</t>
+  </si>
+  <si>
+    <t>Scanning is exited amd total cost is displayed on LCD</t>
+  </si>
+  <si>
+    <t>REQ-12</t>
+  </si>
+  <si>
+    <t>REQ-13</t>
+  </si>
+  <si>
+    <t>REQ-14</t>
+  </si>
+  <si>
+    <t>REQ-15</t>
+  </si>
+  <si>
+    <t>Test that choice of payment is working</t>
+  </si>
+  <si>
+    <t>Code is executing payment portion</t>
+  </si>
+  <si>
+    <t>Press '1' or '2' on LCD</t>
+  </si>
+  <si>
+    <t>REQ-16</t>
+  </si>
+  <si>
+    <t>LCD displays '(Respective payment mode)'</t>
+  </si>
+  <si>
+    <t>Test that payment function has a failsafe if wrong number is entered</t>
+  </si>
+  <si>
+    <t>Press any number != 1 or 2 on keypad</t>
+  </si>
+  <si>
+    <t>LCD displays payment Selector again</t>
+  </si>
+  <si>
+    <t>Scan users card to get UID info and check if balance is sufficent to move forward</t>
+  </si>
+  <si>
+    <t>Tap card on RFID reader</t>
+  </si>
+  <si>
+    <t>Code moves on (no hardware indication</t>
+  </si>
+  <si>
+    <t>Code moves on (no hardware indication)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test that paywave payment is working </t>
+  </si>
+  <si>
+    <t>Test that Pin code payment is working</t>
+  </si>
+  <si>
+    <t>Press 1 on keypad @REQ13</t>
+  </si>
+  <si>
+    <t>Press 2 on keypad @REQ13</t>
+  </si>
+  <si>
+    <t>code finishes payment and LCD displays "Thank you have a nice day"</t>
+  </si>
+  <si>
+    <t>Enter Pin for respectvie Card Scanned  @Req 14 based on datbase</t>
+  </si>
+  <si>
+    <t>LCD displays "Enter Pin" and if Pin is successfully entered displays corect pin and then "Thank you have a nice day"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -163,7 +271,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -186,25 +294,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -221,22 +328,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -248,13 +359,6 @@
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -311,7 +415,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -487,13 +590,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>19</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -565,7 +668,6 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -573,6 +675,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1208,9 +1311,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1248,9 +1351,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1285,7 +1388,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1320,7 +1423,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1493,52 +1596,52 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:C6"/>
   <sheetViews>
-    <sheetView zoomScale="129" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" zoomScale="129" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="6" t="s">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="10">
-        <f>COUNTIF('Test Cases &amp; Results'!B3:B70, "&lt;&gt;")</f>
-        <v>20</v>
+      <c r="C3" s="6">
+        <f>COUNTIF('Test Cases &amp; Results'!B3:B58, "&lt;&gt;")</f>
+        <v>8</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="7" t="s">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="10">
-        <f>COUNTIF('Test Cases &amp; Results'!K3:K72, "Pass")</f>
-        <v>1</v>
+      <c r="C4" s="6">
+        <f>COUNTIF('Test Cases &amp; Results'!K3:K60, "Pass")</f>
+        <v>8</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="8" t="s">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="10">
-        <f>COUNTIF('Test Cases &amp; Results'!K3:K72, "Fail")</f>
+      <c r="C5" s="6">
+        <f>COUNTIF('Test Cases &amp; Results'!K3:K60, "Fail")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="9" t="s">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="10">
-        <f>COUNTIF('Test Cases &amp; Results'!K3:K72, "Not Tested")</f>
-        <v>19</v>
+      <c r="C6" s="6">
+        <f>COUNTIF('Test Cases &amp; Results'!K3:K60, "Not Tested")</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1549,36 +1652,39 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:K22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="B1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="136" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView topLeftCell="A6" zoomScale="136" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="28.140625" customWidth="1"/>
-    <col min="7" max="7" width="21.7109375" customWidth="1"/>
-    <col min="8" max="8" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.42578125" customWidth="1"/>
-    <col min="10" max="10" width="18.5703125" customWidth="1"/>
-    <col min="11" max="11" width="12.5703125" style="13" customWidth="1"/>
+    <col min="6" max="6" width="28.109375" customWidth="1"/>
+    <col min="7" max="7" width="21.6640625" customWidth="1"/>
+    <col min="8" max="8" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.44140625" customWidth="1"/>
+    <col min="10" max="10" width="18.5546875" customWidth="1"/>
+    <col min="11" max="11" width="12.5546875" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="D1" s="9"/>
+    </row>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>5</v>
+      <c r="D2" s="7" t="s">
+        <v>18</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>6</v>
@@ -1598,384 +1704,266 @@
       <c r="J2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="K2" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="2:11" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="2">
+    <row r="3" spans="2:11" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="10">
         <v>1</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="10">
         <v>1</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="K3" s="12" t="s">
+      <c r="I3" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" s="8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="2">
+    <row r="4" spans="2:11" ht="22.8" x14ac:dyDescent="0.3">
+      <c r="B4" s="10">
         <f>B3+1</f>
         <v>2</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="12" t="s">
+      <c r="C4" s="10"/>
+      <c r="D4" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B5" s="10">
+        <f t="shared" ref="B5:B10" si="0">B4+1</f>
         <v>3</v>
       </c>
+      <c r="C5" s="10"/>
+      <c r="D5" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="2">
-        <f t="shared" ref="B5:B20" si="0">B4+1</f>
-        <v>3</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="2">
+    <row r="6" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B6" s="10">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="12" t="s">
-        <v>3</v>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="2">
+    <row r="7" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B7" s="10">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="12" t="s">
-        <v>3</v>
+      <c r="C7" s="11"/>
+      <c r="D7" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="2">
+    <row r="8" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B8" s="10">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="12" t="s">
-        <v>3</v>
+      <c r="C8" s="11"/>
+      <c r="D8" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="J8" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="2">
+    <row r="9" spans="2:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B9" s="10">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="12" t="s">
-        <v>3</v>
+      <c r="C9" s="11"/>
+      <c r="D9" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="J9" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="2">
+    <row r="10" spans="2:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="B10" s="10">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="2">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="2">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="2">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="2">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="2">
-        <f t="shared" si="0"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="2">
-        <f t="shared" si="0"/>
+      <c r="F10" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="J10" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="K10" s="8" t="s">
         <v>14</v>
-      </c>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="2">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="2">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="2">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="2">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B21" s="2">
-        <f t="shared" ref="B21:B22" si="1">B20+1</f>
-        <v>19</v>
-      </c>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="2">
-        <f t="shared" si="1"/>
-        <v>20</v>
-      </c>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="14"/>
-      <c r="K22" s="12" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="K3:K20">
-    <cfRule type="cellIs" dxfId="3" priority="9" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K3:K20">
-    <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
+  <conditionalFormatting sqref="K3:K10">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K21:K22">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"Fail"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K21:K22">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>"Not Tested"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1983,17 +1971,17 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000001000000}">
+          <x14:formula1>
+            <xm:f>Enums!$B$2:$B$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>K3:K10</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{27663CF2-1320-444F-B123-54352C54B6F7}">
           <x14:formula1>
             <xm:f>Enums!$B$8:$B$10</xm:f>
           </x14:formula1>
-          <xm:sqref>E3:E5</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Enums!$B$2:$B$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>K3:K22</xm:sqref>
+          <xm:sqref>E3</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2002,41 +1990,41 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>17</v>
       </c>
@@ -2048,21 +2036,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E81D8C8DDAE8BD44A422697963F06C45" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b6816e004dbb89c674e51f5647972552">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2b02348f-b4e3-458c-83fc-9e90db0f8029" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e6418ca14ac9ee17b8bbf6df78e0c223" ns2:_="">
     <xsd:import namespace="2b02348f-b4e3-458c-83fc-9e90db0f8029"/>
@@ -2220,31 +2193,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69DB72C7-DF0B-4E18-8174-00AB852E6FB4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="2b02348f-b4e3-458c-83fc-9e90db0f8029"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{859B513B-8BED-4B59-B224-E0A2C6173D25}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCDB6385-31B2-4574-9AA4-BF13B563A4E3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2260,4 +2224,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{859B513B-8BED-4B59-B224-E0A2C6173D25}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69DB72C7-DF0B-4E18-8174-00AB852E6FB4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2b02348f-b4e3-458c-83fc-9e90db0f8029"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
All test cases for main page have listed in the excel sheet
</commit_message>
<xml_diff>
--- a/docs/System_Test_Report_template.xlsx
+++ b/docs/System_Test_Report_template.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27830"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83CC02D9-6D26-4B00-A73F-07BC6499151C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{153D5912-0852-432C-9A34-BE24AB2A432B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overall Test Report" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="88">
   <si>
     <t>Total Test Cases</t>
   </si>
@@ -204,6 +204,96 @@
   </si>
   <si>
     <t>LCD displays "Enter Pin" and if Pin is successfully entered displays corect pin and then "Thank you have a nice day"</t>
+  </si>
+  <si>
+    <t>Manual Testing for Website</t>
+  </si>
+  <si>
+    <t xml:space="preserve">             REQ-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expected Result </t>
+  </si>
+  <si>
+    <t>REQ- 1</t>
+  </si>
+  <si>
+    <t>high impact</t>
+  </si>
+  <si>
+    <t>Upon clicking on the product the user should be able to go to the admin page where he/she would be able to select the quantity they would like to purchase</t>
+  </si>
+  <si>
+    <t>Item has been clicked</t>
+  </si>
+  <si>
+    <t>Click on the product</t>
+  </si>
+  <si>
+    <t>Upon clicking on the increase/decrease symbol on the admin page, the customer should be able to increase or decrease they would like to purchase</t>
+  </si>
+  <si>
+    <t>Increase or decrease clicked</t>
+  </si>
+  <si>
+    <t>Click on increase/decrease symbol</t>
+  </si>
+  <si>
+    <t>REQ-2</t>
+  </si>
+  <si>
+    <t>REQ-3</t>
+  </si>
+  <si>
+    <t>moderate impact</t>
+  </si>
+  <si>
+    <t>Upon clicking on the add to cart icon the product should be able to be automatically added to the cart</t>
+  </si>
+  <si>
+    <t>Click on the add to cart button</t>
+  </si>
+  <si>
+    <t>Add to cart button clicked</t>
+  </si>
+  <si>
+    <t>Customer should click on the increase or decrease icon and see that the products quantity is increasing/decreasing</t>
+  </si>
+  <si>
+    <t>Customer clicks on the increase/decrease icon and observers that the quantity is decreasing/increasing</t>
+  </si>
+  <si>
+    <t>Customer is able to be brought directly to the admin page to select the quantity they would like to purchase</t>
+  </si>
+  <si>
+    <t>Once the customer clicks on add to cart button this will add the item to the cart automatically</t>
+  </si>
+  <si>
+    <t>Item automatically gets added to the cart once add to cart icon is clicked</t>
+  </si>
+  <si>
+    <t>REQ-4</t>
+  </si>
+  <si>
+    <t>low impact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Once the customer is satisfied with their purchase they can click on the cart icon to view all the products they have purchased and checkout for payment </t>
+  </si>
+  <si>
+    <t>Cart icon clicked</t>
+  </si>
+  <si>
+    <t>Click on Cart Icon</t>
+  </si>
+  <si>
+    <t>When Cart icon has been clicked, this should show a list of products purchased by the cutomer</t>
+  </si>
+  <si>
+    <t>When cart icon is clicked it shows a list of products purchased by the user</t>
+  </si>
+  <si>
+    <t>Custoemr should be able to be brought directly to the admin page to select the quantity they would like to purchase</t>
   </si>
 </sst>
 </file>
@@ -233,7 +323,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -267,6 +357,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -309,7 +405,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -340,8 +436,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -590,7 +698,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>8</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -1599,34 +1707,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="129" workbookViewId="0">
+    <sheetView zoomScale="129" workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.46484375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="6">
         <f>COUNTIF('Test Cases &amp; Results'!B3:B58, "&lt;&gt;")</f>
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="6">
         <f>COUNTIF('Test Cases &amp; Results'!K3:K60, "Pass")</f>
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
@@ -1635,7 +1743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B6" s="5" t="s">
         <v>3</v>
       </c>
@@ -1653,30 +1761,30 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B1:K10"/>
+  <dimension ref="B1:L19"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="136" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.86328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="28.109375" customWidth="1"/>
+    <col min="6" max="6" width="28.1328125" customWidth="1"/>
     <col min="7" max="7" width="21.6640625" customWidth="1"/>
     <col min="8" max="8" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.44140625" customWidth="1"/>
-    <col min="10" max="10" width="18.5546875" customWidth="1"/>
-    <col min="11" max="11" width="12.5546875" style="9" customWidth="1"/>
+    <col min="9" max="9" width="20.46484375" customWidth="1"/>
+    <col min="10" max="10" width="18.53125" customWidth="1"/>
+    <col min="11" max="11" width="12.53125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:11" x14ac:dyDescent="0.45">
       <c r="D1" s="9"/>
     </row>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1708,7 +1816,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="2:11" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:11" ht="57" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B3" s="10">
         <v>1</v>
       </c>
@@ -1740,7 +1848,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="2:11" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:11" ht="22.5" x14ac:dyDescent="0.45">
       <c r="B4" s="10">
         <f>B3+1</f>
         <v>2</v>
@@ -1771,7 +1879,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:11" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B5" s="10">
         <f t="shared" ref="B5:B10" si="0">B4+1</f>
         <v>3</v>
@@ -1802,7 +1910,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:11" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B6" s="10">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1833,7 +1941,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:11" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B7" s="10">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1864,7 +1972,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:11" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B8" s="10">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1895,7 +2003,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="2:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:11" ht="57" x14ac:dyDescent="0.45">
       <c r="B9" s="10">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1926,7 +2034,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="2:11" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:11" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B10" s="10">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1957,7 +2065,168 @@
         <v>14</v>
       </c>
     </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B13" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B15" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H15" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="I15" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="J15" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="K15" s="15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="B16" s="9">
+        <v>1</v>
+      </c>
+      <c r="C16" s="9"/>
+      <c r="D16" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="I16" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="J16" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="K16" s="16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="B17" s="13">
+        <v>2</v>
+      </c>
+      <c r="C17" s="9"/>
+      <c r="D17" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="G17" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="H17" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="I17" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="J17" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="K17" s="16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" ht="57" x14ac:dyDescent="0.45">
+      <c r="B18" s="13">
+        <v>3</v>
+      </c>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="H18" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="I18" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="J18" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="K18" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="L18" s="13"/>
+    </row>
+    <row r="19" spans="2:12" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="B19" s="13">
+        <v>4</v>
+      </c>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="G19" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="H19" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="I19" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="J19" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="K19" s="17" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B13:D13"/>
+  </mergeCells>
   <conditionalFormatting sqref="K3:K10">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Not Tested"</formula>
@@ -1970,7 +2239,7 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000001000000}">
           <x14:formula1>
             <xm:f>Enums!$B$2:$B$4</xm:f>
@@ -1997,34 +2266,34 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.46484375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B10" t="s">
         <v>17</v>
       </c>
@@ -2036,6 +2305,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E81D8C8DDAE8BD44A422697963F06C45" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b6816e004dbb89c674e51f5647972552">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2b02348f-b4e3-458c-83fc-9e90db0f8029" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e6418ca14ac9ee17b8bbf6df78e0c223" ns2:_="">
     <xsd:import namespace="2b02348f-b4e3-458c-83fc-9e90db0f8029"/>
@@ -2193,22 +2477,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69DB72C7-DF0B-4E18-8174-00AB852E6FB4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2b02348f-b4e3-458c-83fc-9e90db0f8029"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{859B513B-8BED-4B59-B224-E0A2C6173D25}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCDB6385-31B2-4574-9AA4-BF13B563A4E3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2224,28 +2517,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{859B513B-8BED-4B59-B224-E0A2C6173D25}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69DB72C7-DF0B-4E18-8174-00AB852E6FB4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="2b02348f-b4e3-458c-83fc-9e90db0f8029"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>